<commit_message>
fix: graph for analysis
</commit_message>
<xml_diff>
--- a/analysis/Summary.xlsx
+++ b/analysis/Summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/naufal_hardiansyah_binus_edu/Documents/Documents/UNMC/Artificial Intelligence Methods/Project_/Bin-Packing-Problem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://binusianorg-my.sharepoint.com/personal/naufal_hardiansyah_binus_edu/Documents/Documents/UNMC/Artificial Intelligence Methods/Project_/Bin-Packing-Problem/analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{59498A66-809D-43BB-BBD7-6024243EEA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{59498A66-809D-43BB-BBD7-6024243EEA8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E067E470-47B0-4E8E-B327-2965CFF95DD1}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,11 +17,24 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
     <sheet name="summary" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
     <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -563,9 +576,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -740,87 +754,139 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>summary!$A$2:$B$21</c:f>
+              <c:f>summary!$A$3:$B$22</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>FA</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>TS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="4">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="5">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
                     <c:v>TS</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="7">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="8">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="10">
                     <c:v>TS</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="11">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="13">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="14">
                     <c:v>TS</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="15">
-                    <c:v>TS</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>MFFD</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>GA</c:v>
-                  </c:pt>
                   <c:pt idx="18">
-                    <c:v>FA</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
                     <c:v>TS</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>TEST0082</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="3">
                     <c:v>TEST0030</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="7">
                     <c:v>TEST0044</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="11">
                     <c:v>TEST0014</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="15">
                     <c:v>TEST0049</c:v>
                   </c:pt>
                 </c:lvl>
@@ -829,68 +895,65 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>summary!$C$2:$C$21</c:f>
+              <c:f>summary!$C$3:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>30.966999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30.966999999999999</c:v>
+                  <c:v>27.4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>27.4</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>32.633000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>32.633000000000003</c:v>
+                  <c:v>29.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29.9</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>15.433</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>15</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>15.433</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>14</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>15</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24</c:v>
+                  <c:v>27.7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.7</c:v>
+                  <c:v>25.033000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25.033000000000001</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12</c:v>
+                  <c:v>12.032999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12.032999999999999</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
@@ -926,87 +989,139 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>summary!$A$2:$B$21</c:f>
+              <c:f>summary!$A$3:$B$22</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="20"/>
+                <c:ptCount val="19"/>
                 <c:lvl>
                   <c:pt idx="0">
+                    <c:v>GA</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>FA</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>TS</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="1">
+                  <c:pt idx="4">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="2">
+                  <c:pt idx="5">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="3">
+                  <c:pt idx="6">
                     <c:v>TS</c:v>
                   </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="7">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="5">
+                  <c:pt idx="8">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="6">
+                  <c:pt idx="9">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="7">
+                  <c:pt idx="10">
                     <c:v>TS</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="11">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="9">
+                  <c:pt idx="12">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="10">
+                  <c:pt idx="13">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="11">
+                  <c:pt idx="14">
                     <c:v>TS</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="15">
                     <c:v>MFFD</c:v>
                   </c:pt>
-                  <c:pt idx="13">
+                  <c:pt idx="16">
                     <c:v>GA</c:v>
                   </c:pt>
-                  <c:pt idx="14">
+                  <c:pt idx="17">
                     <c:v>FA</c:v>
                   </c:pt>
-                  <c:pt idx="15">
-                    <c:v>TS</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>MFFD</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>GA</c:v>
-                  </c:pt>
                   <c:pt idx="18">
-                    <c:v>FA</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
                     <c:v>TS</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>TEST0082</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
+                  <c:pt idx="3">
                     <c:v>TEST0030</c:v>
                   </c:pt>
-                  <c:pt idx="8">
+                  <c:pt idx="7">
                     <c:v>TEST0044</c:v>
                   </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="11">
                     <c:v>TEST0014</c:v>
                   </c:pt>
-                  <c:pt idx="16">
+                  <c:pt idx="15">
                     <c:v>TEST0049</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1015,68 +1130,65 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>summary!$D$2:$D$21</c:f>
+              <c:f>summary!$D$3:$D$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>95.881</c:v>
+                  <c:v>77.457999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.457999999999998</c:v>
+                  <c:v>84.775999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>84.775999999999996</c:v>
+                  <c:v>77.429000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>77.429000000000002</c:v>
+                  <c:v>96.415999999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>96.415999999999997</c:v>
+                  <c:v>82.781000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>82.781000000000006</c:v>
+                  <c:v>87.570999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87.570999999999998</c:v>
+                  <c:v>84.444000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84.444000000000003</c:v>
+                  <c:v>93.325999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>93.325999999999993</c:v>
+                  <c:v>90.798000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90.798000000000002</c:v>
+                  <c:v>93.988</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>93.988</c:v>
+                  <c:v>91.981999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>91.981999999999999</c:v>
+                  <c:v>95.820999999999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>95.820999999999998</c:v>
+                  <c:v>83.081000000000003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>83.081000000000003</c:v>
+                  <c:v>88.608000000000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>88.608000000000004</c:v>
+                  <c:v>84.82</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>84.82</c:v>
+                  <c:v>91.617000000000004</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>91.617000000000004</c:v>
+                  <c:v>91.382000000000005</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>91.382000000000005</c:v>
+                  <c:v>93.594999999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>93.594999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
                   <c:v>94.688999999999993</c:v>
                 </c:pt>
               </c:numCache>
@@ -1089,8 +1201,9 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1133,93 +1246,145 @@
                   <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>summary!$A$2:$B$21</c15:sqref>
+                          <c15:sqref>summary!$A$3:$B$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="20"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
+                          <c:v>GA</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>FA</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>TS</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="1">
+                        <c:pt idx="4">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="2">
+                        <c:pt idx="5">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="3">
+                        <c:pt idx="6">
                           <c:v>TS</c:v>
                         </c:pt>
-                        <c:pt idx="4">
+                        <c:pt idx="7">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="5">
+                        <c:pt idx="8">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="6">
+                        <c:pt idx="9">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="7">
+                        <c:pt idx="10">
                           <c:v>TS</c:v>
                         </c:pt>
-                        <c:pt idx="8">
+                        <c:pt idx="11">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="9">
+                        <c:pt idx="12">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="10">
+                        <c:pt idx="13">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="11">
+                        <c:pt idx="14">
                           <c:v>TS</c:v>
                         </c:pt>
-                        <c:pt idx="12">
+                        <c:pt idx="15">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="13">
+                        <c:pt idx="16">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="14">
+                        <c:pt idx="17">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="15">
-                          <c:v>TS</c:v>
-                        </c:pt>
-                        <c:pt idx="16">
-                          <c:v>MFFD</c:v>
-                        </c:pt>
-                        <c:pt idx="17">
-                          <c:v>GA</c:v>
-                        </c:pt>
                         <c:pt idx="18">
-                          <c:v>FA</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
                           <c:v>TS</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
-                        <c:pt idx="0">
-                          <c:v>TEST0082</c:v>
-                        </c:pt>
-                        <c:pt idx="4">
+                        <c:pt idx="3">
                           <c:v>TEST0030</c:v>
                         </c:pt>
-                        <c:pt idx="8">
+                        <c:pt idx="7">
                           <c:v>TEST0044</c:v>
                         </c:pt>
-                        <c:pt idx="12">
+                        <c:pt idx="11">
                           <c:v>TEST0014</c:v>
                         </c:pt>
-                        <c:pt idx="16">
+                        <c:pt idx="15">
                           <c:v>TEST0049</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1231,71 +1396,68 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>summary!$E$2:$E$21</c15:sqref>
+                          <c15:sqref>summary!$E$3:$E$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>General</c:formatCode>
+                      <c:formatCode>0.00</c:formatCode>
                       <c:ptCount val="20"/>
                       <c:pt idx="0">
-                        <c:v>0.154</c:v>
+                        <c:v>0.161</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>0.161</c:v>
+                        <c:v>0.13200000000000001</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>0.13200000000000001</c:v>
+                        <c:v>0.156</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>0.156</c:v>
+                        <c:v>0.153</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>0.153</c:v>
+                        <c:v>0.123</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>0.123</c:v>
+                        <c:v>9.7000000000000003E-2</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>9.7000000000000003E-2</c:v>
+                        <c:v>0.109</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>0.109</c:v>
+                        <c:v>0.24199999999999999</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.24199999999999999</c:v>
+                        <c:v>0.11700000000000001</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>0.11700000000000001</c:v>
+                        <c:v>4.8000000000000001E-2</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>4.8000000000000001E-2</c:v>
+                        <c:v>5.8000000000000003E-2</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>5.8000000000000003E-2</c:v>
+                        <c:v>0.17</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>0.17</c:v>
+                        <c:v>0.13</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>0.13</c:v>
+                        <c:v>9.1999999999999998E-2</c:v>
                       </c:pt>
                       <c:pt idx="14">
+                        <c:v>8.2000000000000003E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.27100000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
                         <c:v>9.1999999999999998E-2</c:v>
                       </c:pt>
-                      <c:pt idx="15">
-                        <c:v>8.2000000000000003E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>0.27100000000000002</c:v>
-                      </c:pt>
                       <c:pt idx="17">
-                        <c:v>9.1999999999999998E-2</c:v>
+                        <c:v>4.7E-2</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>4.7E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
                         <c:v>3.7999999999999999E-2</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1314,7 +1476,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>summary!$F$1</c15:sqref>
@@ -1339,93 +1501,145 @@
                   <a:effectLst/>
                 </c:spPr>
                 <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="75000"/>
+                              <a:lumOff val="25000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                            <a:round/>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
                 <c:cat>
                   <c:multiLvlStrRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>summary!$A$2:$B$21</c15:sqref>
+                          <c15:sqref>summary!$A$3:$B$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="20"/>
+                      <c:ptCount val="19"/>
                       <c:lvl>
                         <c:pt idx="0">
+                          <c:v>GA</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>FA</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>TS</c:v>
+                        </c:pt>
+                        <c:pt idx="3">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="1">
+                        <c:pt idx="4">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="2">
+                        <c:pt idx="5">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="3">
+                        <c:pt idx="6">
                           <c:v>TS</c:v>
                         </c:pt>
-                        <c:pt idx="4">
+                        <c:pt idx="7">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="5">
+                        <c:pt idx="8">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="6">
+                        <c:pt idx="9">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="7">
+                        <c:pt idx="10">
                           <c:v>TS</c:v>
                         </c:pt>
-                        <c:pt idx="8">
+                        <c:pt idx="11">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="9">
+                        <c:pt idx="12">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="10">
+                        <c:pt idx="13">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="11">
+                        <c:pt idx="14">
                           <c:v>TS</c:v>
                         </c:pt>
-                        <c:pt idx="12">
+                        <c:pt idx="15">
                           <c:v>MFFD</c:v>
                         </c:pt>
-                        <c:pt idx="13">
+                        <c:pt idx="16">
                           <c:v>GA</c:v>
                         </c:pt>
-                        <c:pt idx="14">
+                        <c:pt idx="17">
                           <c:v>FA</c:v>
                         </c:pt>
-                        <c:pt idx="15">
-                          <c:v>TS</c:v>
-                        </c:pt>
-                        <c:pt idx="16">
-                          <c:v>MFFD</c:v>
-                        </c:pt>
-                        <c:pt idx="17">
-                          <c:v>GA</c:v>
-                        </c:pt>
                         <c:pt idx="18">
-                          <c:v>FA</c:v>
-                        </c:pt>
-                        <c:pt idx="19">
                           <c:v>TS</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
-                        <c:pt idx="0">
-                          <c:v>TEST0082</c:v>
-                        </c:pt>
-                        <c:pt idx="4">
+                        <c:pt idx="3">
                           <c:v>TEST0030</c:v>
                         </c:pt>
-                        <c:pt idx="8">
+                        <c:pt idx="7">
                           <c:v>TEST0044</c:v>
                         </c:pt>
-                        <c:pt idx="12">
+                        <c:pt idx="11">
                           <c:v>TEST0014</c:v>
                         </c:pt>
-                        <c:pt idx="16">
+                        <c:pt idx="15">
                           <c:v>TEST0049</c:v>
                         </c:pt>
                       </c:lvl>
@@ -1434,10 +1648,10 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>summary!$F$2:$F$21</c15:sqref>
+                          <c15:sqref>summary!$F$3:$F$22</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1445,63 +1659,60 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="20"/>
                       <c:pt idx="0">
+                        <c:v>27.466999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>226.36699999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>40.933</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>3.3000000000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>45.933</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>225.5</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>21.632999999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
                         <c:v>0.1</c:v>
                       </c:pt>
-                      <c:pt idx="1">
-                        <c:v>27.466999999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>226.36699999999999</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>40.933</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>3.3000000000000002E-2</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>45.933</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>225.5</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>21.632999999999999</c:v>
-                      </c:pt>
                       <c:pt idx="8">
-                        <c:v>0.1</c:v>
+                        <c:v>44.832999999999998</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>44.832999999999998</c:v>
+                        <c:v>258.06700000000001</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>258.06700000000001</c:v>
+                        <c:v>13.5</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>13.5</c:v>
+                        <c:v>6.7000000000000004E-2</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>6.7000000000000004E-2</c:v>
+                        <c:v>38.9</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>38.9</c:v>
+                        <c:v>194.7</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>194.7</c:v>
+                        <c:v>19.033000000000001</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>19.033000000000001</c:v>
+                        <c:v>0.33300000000000002</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>0.33300000000000002</c:v>
+                        <c:v>37.1</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>37.1</c:v>
+                        <c:v>23.6</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>23.6</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
                         <c:v>18.899999999999999</c:v>
                       </c:pt>
                     </c:numCache>
@@ -2173,37 +2384,8 @@
       <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
-  <c:pivotSource>
-    <c:name>[summary.xlsx]Sheet2!PivotTable24</c:name>
-    <c:fmtId val="3"/>
-  </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Sum of  Avg. Fairness of Packing by Algorithm</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2234,176 +2416,6 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
-    <c:pivotFmts>
-      <c:pivotFmt>
-        <c:idx val="0"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="1"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-      <c:pivotFmt>
-        <c:idx val="2"/>
-        <c:spPr>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:marker>
-          <c:symbol val="none"/>
-        </c:marker>
-        <c:dLbl>
-          <c:idx val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-          </c:extLst>
-        </c:dLbl>
-      </c:pivotFmt>
-    </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2415,11 +2427,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$B$3</c:f>
+              <c:f>summary!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Total</c:v>
+                  <c:v> Avg. Fairness of Packing</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2434,56 +2446,230 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet2!$A$4:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>FA</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>GA</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>MFF</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>TS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>summary!$A$2:$B$21</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>MFFD</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>GA</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>FA</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>TS</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>MFFD</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>GA</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>FA</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>TS</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>MFFD</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>GA</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>FA</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>TS</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>MFFD</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>GA</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>FA</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>TS</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>MFFD</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>GA</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>FA</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>TS</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>TEST0082</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>TEST0030</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>TEST0044</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>TEST0014</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>TEST0049</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$B$4:$B$7</c:f>
+              <c:f>summary!$E$2:$E$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.41299999999999998</c:v>
+                  <c:v>0.154</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.626</c:v>
+                  <c:v>0.161</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.99</c:v>
+                  <c:v>0.13200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.442</c:v>
+                  <c:v>0.156</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.153</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.123</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.7000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.109</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.24199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.11700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.8000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.2000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.27100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.1999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4BE9-44F3-99C0-9ED0F29DD8DD}"/>
+              <c16:uniqueId val="{00000000-C196-447C-9C36-99E18737C19D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -2491,11 +2677,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1226000159"/>
-        <c:axId val="1226014559"/>
+        <c:axId val="1326914303"/>
+        <c:axId val="1326904703"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1226000159"/>
+        <c:axId val="1326914303"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2538,7 +2724,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1226014559"/>
+        <c:crossAx val="1326904703"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2546,7 +2732,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1226014559"/>
+        <c:axId val="1326904703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2566,7 +2752,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2597,49 +2783,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1226000159"/>
+        <c:crossAx val="1326914303"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
-      <c:dTable>
-        <c:showHorzBorder val="1"/>
-        <c:showVertBorder val="1"/>
-        <c:showOutline val="1"/>
-        <c:showKeys val="1"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr rtl="0">
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -2650,6 +2797,13 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2682,21 +2836,6 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
-  <c:extLst>
-    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
-      <c14:pivotOptions>
-        <c14:dropZoneFilter val="1"/>
-        <c14:dropZoneCategories val="1"/>
-        <c14:dropZoneData val="1"/>
-        <c14:dropZonesVisible val="1"/>
-      </c14:pivotOptions>
-    </c:ext>
-    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
-      <c16:pivotOptions16>
-        <c16:showExpandCollapseFieldButtons val="1"/>
-      </c16:pivotOptions16>
-    </c:ext>
-  </c:extLst>
 </c:chartSpace>
 </file>
 
@@ -4335,14 +4474,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>15089</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>35527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>490396</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>112646</xdr:rowOff>
     </xdr:to>
@@ -4408,28 +4547,26 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>392546</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>23091</xdr:rowOff>
+      <xdr:colOff>497416</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>20108</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>76589</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>50250</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>148166</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>64558</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7721321C-DEAF-4D37-9245-6DBD08A22FEB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93795CF-BBE5-F9C3-F75F-0E9EC77C1E1B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4444,10 +4581,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5567,10 +5700,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
+      <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5613,10 +5746,10 @@
       <c r="C2">
         <v>25</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>95.881</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>0.154</v>
       </c>
       <c r="F2">
@@ -5633,10 +5766,10 @@
       <c r="C3">
         <v>30.966999999999999</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>77.457999999999998</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.161</v>
       </c>
       <c r="F3">
@@ -5653,10 +5786,10 @@
       <c r="C4">
         <v>27.4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>84.775999999999996</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.13200000000000001</v>
       </c>
       <c r="F4">
@@ -5673,10 +5806,10 @@
       <c r="C5">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>77.429000000000002</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.156</v>
       </c>
       <c r="F5">
@@ -5696,10 +5829,10 @@
       <c r="C6">
         <v>28</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>96.415999999999997</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.153</v>
       </c>
       <c r="F6">
@@ -5716,10 +5849,10 @@
       <c r="C7">
         <v>32.633000000000003</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>82.781000000000006</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.123</v>
       </c>
       <c r="F7">
@@ -5736,10 +5869,10 @@
       <c r="C8">
         <v>29.9</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>87.570999999999998</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>9.7000000000000003E-2</v>
       </c>
       <c r="F8">
@@ -5756,10 +5889,10 @@
       <c r="C9">
         <v>31</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>84.444000000000003</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>0.109</v>
       </c>
       <c r="F9">
@@ -5779,10 +5912,10 @@
       <c r="C10">
         <v>15</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>93.325999999999993</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.24199999999999999</v>
       </c>
       <c r="F10">
@@ -5799,10 +5932,10 @@
       <c r="C11">
         <v>15.433</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>90.798000000000002</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>0.11700000000000001</v>
       </c>
       <c r="F11">
@@ -5819,10 +5952,10 @@
       <c r="C12">
         <v>14</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>93.988</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="F12">
@@ -5839,10 +5972,10 @@
       <c r="C13">
         <v>15</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>91.981999999999999</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="F13">
@@ -5862,10 +5995,10 @@
       <c r="C14">
         <v>24</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>95.820999999999998</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>0.17</v>
       </c>
       <c r="F14">
@@ -5882,10 +6015,10 @@
       <c r="C15">
         <v>27.7</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>83.081000000000003</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>0.13</v>
       </c>
       <c r="F15">
@@ -5902,10 +6035,10 @@
       <c r="C16">
         <v>25.033000000000001</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>88.608000000000004</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="2">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F16">
@@ -5922,10 +6055,10 @@
       <c r="C17">
         <v>27</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>84.82</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="F17">
@@ -5945,10 +6078,10 @@
       <c r="C18">
         <v>12</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>91.617000000000004</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>0.27100000000000002</v>
       </c>
       <c r="F18">
@@ -5965,10 +6098,10 @@
       <c r="C19">
         <v>12.032999999999999</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>91.382000000000005</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>9.1999999999999998E-2</v>
       </c>
       <c r="F19">
@@ -5985,10 +6118,10 @@
       <c r="C20">
         <v>11</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>93.594999999999999</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>4.7E-2</v>
       </c>
       <c r="F20">
@@ -6005,10 +6138,10 @@
       <c r="C21">
         <v>11</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>94.688999999999993</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="F21">
@@ -6016,6 +6149,16 @@
       </c>
       <c r="G21">
         <v>567</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <f>E4+E8+E12+E16+E20</f>
+        <v>0.41599999999999998</v>
+      </c>
+      <c r="D31">
+        <f>E2+E6+E10+E14+E18</f>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>